<commit_message>
testFile.xlsx, modify abdul khan swipe in 0605(late)
</commit_message>
<xml_diff>
--- a/src/main/resources/testFile.xlsx
+++ b/src/main/resources/testFile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="68">
   <si>
     <t xml:space="preserve">Report Title:</t>
   </si>
@@ -433,13 +433,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H116"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.85"/>
@@ -542,15 +542,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>44324.2379050926</v>
+        <v>44324.2536342593</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
@@ -576,7 +576,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>44324.238599537</v>
+        <v>44324.6619560185</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>20</v>
@@ -585,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>22</v>
@@ -602,7 +602,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>44324.4098842593</v>
+        <v>44324.7394560185</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>20</v>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>22</v>
@@ -620,7 +620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -628,7 +628,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>44324.6619560185</v>
+        <v>44324.7423726852</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>20</v>
@@ -637,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>22</v>
@@ -646,7 +646,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -654,7 +654,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>44324.7394560185</v>
+        <v>44325.2423611111</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>20</v>
@@ -672,15 +672,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>44324.7423726852</v>
+        <v>44324.2404861111</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>20</v>
@@ -700,13 +700,13 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>44325.2423611111</v>
+        <v>44324.75</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>20</v>
@@ -715,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>22</v>
@@ -724,15 +724,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>44325.2359143519</v>
+        <v>44324.7359837963</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>20</v>
@@ -741,7 +741,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>22</v>
@@ -758,7 +758,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>44324.2404861111</v>
+        <v>44324.8191550926</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>20</v>
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>22</v>
@@ -784,7 +784,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>44324.7352893519</v>
+        <v>44324.8323263889</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>20</v>
@@ -793,7 +793,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>22</v>
@@ -810,7 +810,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>44324.7359837963</v>
+        <v>44325.0769791667</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>20</v>
@@ -836,7 +836,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>44324.8191550926</v>
+        <v>44325.09125</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
@@ -845,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>22</v>
@@ -862,7 +862,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="3" t="n">
-        <v>44324.8323263889</v>
+        <v>44325.2371180556</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>20</v>
@@ -882,13 +882,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C22" s="3" t="n">
-        <v>44325.0769791667</v>
+        <v>44324.2481365741</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>20</v>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>22</v>
@@ -906,15 +906,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3" t="n">
-        <v>44325.09125</v>
+        <v>44324.2919328704</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>20</v>
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>22</v>
@@ -934,13 +934,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>44325.2371180556</v>
+        <v>44324.7502662037</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>20</v>
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>22</v>
@@ -966,7 +966,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="3" t="n">
-        <v>44324.2481365741</v>
+        <v>44325.2498611111</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>20</v>
@@ -992,7 +992,7 @@
         <v>30</v>
       </c>
       <c r="C26" s="3" t="n">
-        <v>44324.2919328704</v>
+        <v>44325.7498611111</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>20</v>
@@ -1001,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>22</v>
@@ -1012,19 +1012,19 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C27" s="3" t="n">
-        <v>44324.7502662037</v>
+        <v>44324.246412037</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>32</v>
@@ -1033,24 +1033,24 @@
         <v>22</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C28" s="3" t="n">
-        <v>44325.2498611111</v>
+        <v>44324.7481134259</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>31</v>
@@ -1059,24 +1059,24 @@
         <v>22</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3" t="n">
-        <v>44325.7498611111</v>
+        <v>44324.7514467593</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>31</v>
@@ -1085,7 +1085,7 @@
         <v>22</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,7 +1096,7 @@
         <v>34</v>
       </c>
       <c r="C30" s="3" t="n">
-        <v>44324.246412037</v>
+        <v>44325.2491550926</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>20</v>
@@ -1116,19 +1116,19 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C31" s="3" t="n">
-        <v>44324.7481134259</v>
+        <v>44324.2345601852</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>31</v>
@@ -1137,59 +1137,59 @@
         <v>22</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C32" s="3" t="n">
-        <v>44324.7514467593</v>
+        <v>44324.7356944444</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C33" s="3" t="n">
-        <v>44325.2491550926</v>
+        <v>44324.739375</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1200,7 +1200,7 @@
         <v>38</v>
       </c>
       <c r="C34" s="3" t="n">
-        <v>44324.2345601852</v>
+        <v>44324.8677314815</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>20</v>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>22</v>
@@ -1226,7 +1226,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="3" t="n">
-        <v>44324.7356944444</v>
+        <v>44324.8735416667</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>20</v>
@@ -1235,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>22</v>
@@ -1252,7 +1252,7 @@
         <v>38</v>
       </c>
       <c r="C36" s="3" t="n">
-        <v>44324.739375</v>
+        <v>44324.8756018519</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>20</v>
@@ -1261,7 +1261,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>22</v>
@@ -1278,7 +1278,7 @@
         <v>38</v>
       </c>
       <c r="C37" s="3" t="n">
-        <v>44324.8677314815</v>
+        <v>44324.8761805556</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>20</v>
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>22</v>
@@ -1304,7 +1304,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="3" t="n">
-        <v>44324.8735416667</v>
+        <v>44324.8838773148</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>20</v>
@@ -1313,7 +1313,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>22</v>
@@ -1330,7 +1330,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="3" t="n">
-        <v>44324.8756018519</v>
+        <v>44324.8871643519</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>20</v>
@@ -1339,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>22</v>
@@ -1356,7 +1356,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="3" t="n">
-        <v>44324.8761805556</v>
+        <v>44324.891087963</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>20</v>
@@ -1365,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>22</v>
@@ -1382,7 +1382,7 @@
         <v>38</v>
       </c>
       <c r="C41" s="3" t="n">
-        <v>44324.8838773148</v>
+        <v>44324.8930671296</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>20</v>
@@ -1391,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>22</v>
@@ -1408,7 +1408,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="3" t="n">
-        <v>44324.8871643519</v>
+        <v>44324.8947337963</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>20</v>
@@ -1417,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>22</v>
@@ -1434,7 +1434,7 @@
         <v>38</v>
       </c>
       <c r="C43" s="3" t="n">
-        <v>44324.891087963</v>
+        <v>44324.9606481481</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>20</v>
@@ -1443,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>22</v>
@@ -1460,7 +1460,7 @@
         <v>38</v>
       </c>
       <c r="C44" s="3" t="n">
-        <v>44324.8930671296</v>
+        <v>44324.9623611111</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>20</v>
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>22</v>
@@ -1486,7 +1486,7 @@
         <v>38</v>
       </c>
       <c r="C45" s="3" t="n">
-        <v>44324.8947337963</v>
+        <v>44324.9653703704</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>20</v>
@@ -1495,7 +1495,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>22</v>
@@ -1512,7 +1512,7 @@
         <v>38</v>
       </c>
       <c r="C46" s="3" t="n">
-        <v>44324.9606481481</v>
+        <v>44324.9690509259</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>20</v>
@@ -1521,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>22</v>
@@ -1538,7 +1538,7 @@
         <v>38</v>
       </c>
       <c r="C47" s="3" t="n">
-        <v>44324.9623611111</v>
+        <v>44324.974375</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>20</v>
@@ -1547,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>22</v>
@@ -1564,7 +1564,7 @@
         <v>38</v>
       </c>
       <c r="C48" s="3" t="n">
-        <v>44324.9653703704</v>
+        <v>44325.0288425926</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>20</v>
@@ -1573,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>22</v>
@@ -1590,7 +1590,7 @@
         <v>38</v>
       </c>
       <c r="C49" s="3" t="n">
-        <v>44324.9690509259</v>
+        <v>44325.1437268518</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>20</v>
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>22</v>
@@ -1616,7 +1616,7 @@
         <v>38</v>
       </c>
       <c r="C50" s="3" t="n">
-        <v>44324.974375</v>
+        <v>44325.1486458333</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>20</v>
@@ -1625,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>22</v>
@@ -1642,7 +1642,7 @@
         <v>38</v>
       </c>
       <c r="C51" s="3" t="n">
-        <v>44325.0288425926</v>
+        <v>44325.1714814815</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>20</v>
@@ -1651,7 +1651,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>22</v>
@@ -1668,7 +1668,7 @@
         <v>38</v>
       </c>
       <c r="C52" s="3" t="n">
-        <v>44325.1437268518</v>
+        <v>44325.1767013889</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>20</v>
@@ -1677,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>22</v>
@@ -1694,7 +1694,7 @@
         <v>38</v>
       </c>
       <c r="C53" s="3" t="n">
-        <v>44325.1486458333</v>
+        <v>44325.177349537</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>20</v>
@@ -1703,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>22</v>
@@ -1720,7 +1720,7 @@
         <v>38</v>
       </c>
       <c r="C54" s="3" t="n">
-        <v>44325.1714814815</v>
+        <v>44325.1797337963</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>20</v>
@@ -1729,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>22</v>
@@ -1746,7 +1746,7 @@
         <v>38</v>
       </c>
       <c r="C55" s="3" t="n">
-        <v>44325.1767013889</v>
+        <v>44325.1814236111</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>20</v>
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>22</v>
@@ -1772,7 +1772,7 @@
         <v>38</v>
       </c>
       <c r="C56" s="3" t="n">
-        <v>44325.177349537</v>
+        <v>44325.1848148148</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>20</v>
@@ -1781,7 +1781,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>22</v>
@@ -1798,7 +1798,7 @@
         <v>38</v>
       </c>
       <c r="C57" s="3" t="n">
-        <v>44325.1797337963</v>
+        <v>44325.1870138889</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>20</v>
@@ -1807,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>22</v>
@@ -1824,7 +1824,7 @@
         <v>38</v>
       </c>
       <c r="C58" s="3" t="n">
-        <v>44325.1814236111</v>
+        <v>44325.1889814815</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>20</v>
@@ -1833,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>22</v>
@@ -1850,7 +1850,7 @@
         <v>38</v>
       </c>
       <c r="C59" s="3" t="n">
-        <v>44325.1848148148</v>
+        <v>44325.2369791667</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>20</v>
@@ -1859,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>22</v>
@@ -1870,13 +1870,13 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C60" s="3" t="n">
-        <v>44325.1870138889</v>
+        <v>44324.2438310185</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>20</v>
@@ -1885,7 +1885,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>22</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C61" s="3" t="n">
-        <v>44325.1889814815</v>
+        <v>44324.7376388889</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>20</v>
@@ -1911,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>22</v>
@@ -1922,13 +1922,13 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C62" s="3" t="n">
-        <v>44325.2369791667</v>
+        <v>44325.2382986111</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>20</v>
@@ -1937,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>22</v>
@@ -1948,80 +1948,80 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C63" s="3" t="n">
-        <v>44324.2438310185</v>
+        <v>44324.2443171296</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C64" s="3" t="n">
-        <v>44324.7376388889</v>
+        <v>44324.248912037</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C65" s="3" t="n">
-        <v>44325.2382986111</v>
+        <v>44324.7090856481</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,7 +2032,7 @@
         <v>63</v>
       </c>
       <c r="C66" s="3" t="n">
-        <v>44324.2443171296</v>
+        <v>44324.7258796296</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>20</v>
@@ -2041,7 +2041,7 @@
         <v>35</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>22</v>
@@ -2058,7 +2058,7 @@
         <v>63</v>
       </c>
       <c r="C67" s="3" t="n">
-        <v>44324.248912037</v>
+        <v>44325.2415046296</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>20</v>
@@ -2067,7 +2067,7 @@
         <v>35</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>22</v>
@@ -2084,7 +2084,7 @@
         <v>63</v>
       </c>
       <c r="C68" s="3" t="n">
-        <v>44324.7090856481</v>
+        <v>44325.2459837963</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>20</v>
@@ -2093,7 +2093,7 @@
         <v>35</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>22</v>
@@ -2104,80 +2104,80 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C69" s="3" t="n">
-        <v>44324.7258796296</v>
+        <v>44324.2283101852</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C70" s="3" t="n">
-        <v>44325.2415046296</v>
+        <v>44324.2298611111</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C71" s="3" t="n">
-        <v>44325.2459837963</v>
+        <v>44324.2525</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,7 +2188,7 @@
         <v>65</v>
       </c>
       <c r="C72" s="3" t="n">
-        <v>44324.2283101852</v>
+        <v>44324.2533564815</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>20</v>
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>22</v>
@@ -2214,7 +2214,7 @@
         <v>65</v>
       </c>
       <c r="C73" s="3" t="n">
-        <v>44324.2298611111</v>
+        <v>44324.2536458333</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>20</v>
@@ -2223,7 +2223,7 @@
         <v>1</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>22</v>
@@ -2240,7 +2240,7 @@
         <v>65</v>
       </c>
       <c r="C74" s="3" t="n">
-        <v>44324.2525</v>
+        <v>44324.2545601852</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>20</v>
@@ -2249,7 +2249,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>22</v>
@@ -2266,7 +2266,7 @@
         <v>65</v>
       </c>
       <c r="C75" s="3" t="n">
-        <v>44324.2533564815</v>
+        <v>44324.2553472222</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>20</v>
@@ -2275,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>22</v>
@@ -2292,7 +2292,7 @@
         <v>65</v>
       </c>
       <c r="C76" s="3" t="n">
-        <v>44324.2536458333</v>
+        <v>44324.2562152778</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>20</v>
@@ -2301,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>22</v>
@@ -2318,7 +2318,7 @@
         <v>65</v>
       </c>
       <c r="C77" s="3" t="n">
-        <v>44324.2545601852</v>
+        <v>44324.3742013889</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>20</v>
@@ -2327,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>22</v>
@@ -2344,7 +2344,7 @@
         <v>65</v>
       </c>
       <c r="C78" s="3" t="n">
-        <v>44324.2553472222</v>
+        <v>44324.375625</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>20</v>
@@ -2353,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>22</v>
@@ -2370,7 +2370,7 @@
         <v>65</v>
       </c>
       <c r="C79" s="3" t="n">
-        <v>44324.2562152778</v>
+        <v>44324.3760416667</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>20</v>
@@ -2379,7 +2379,7 @@
         <v>1</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>22</v>
@@ -2396,7 +2396,7 @@
         <v>65</v>
       </c>
       <c r="C80" s="3" t="n">
-        <v>44324.3742013889</v>
+        <v>44324.3765393519</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>20</v>
@@ -2405,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>22</v>
@@ -2422,7 +2422,7 @@
         <v>65</v>
       </c>
       <c r="C81" s="3" t="n">
-        <v>44324.375625</v>
+        <v>44324.3770138889</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>20</v>
@@ -2431,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>22</v>
@@ -2448,7 +2448,7 @@
         <v>65</v>
       </c>
       <c r="C82" s="3" t="n">
-        <v>44324.3760416667</v>
+        <v>44324.3917592593</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>20</v>
@@ -2457,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>22</v>
@@ -2474,7 +2474,7 @@
         <v>65</v>
       </c>
       <c r="C83" s="3" t="n">
-        <v>44324.3765393519</v>
+        <v>44324.3940625</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>20</v>
@@ -2483,7 +2483,7 @@
         <v>1</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>22</v>
@@ -2500,7 +2500,7 @@
         <v>65</v>
       </c>
       <c r="C84" s="3" t="n">
-        <v>44324.3770138889</v>
+        <v>44324.3952314815</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>20</v>
@@ -2509,7 +2509,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>22</v>
@@ -2526,7 +2526,7 @@
         <v>65</v>
       </c>
       <c r="C85" s="3" t="n">
-        <v>44324.3917592593</v>
+        <v>44324.3985532407</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>20</v>
@@ -2535,7 +2535,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>22</v>
@@ -2552,7 +2552,7 @@
         <v>65</v>
       </c>
       <c r="C86" s="3" t="n">
-        <v>44324.3940625</v>
+        <v>44324.4017361111</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>20</v>
@@ -2561,7 +2561,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>22</v>
@@ -2578,7 +2578,7 @@
         <v>65</v>
       </c>
       <c r="C87" s="3" t="n">
-        <v>44324.3952314815</v>
+        <v>44324.4025578704</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>20</v>
@@ -2587,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>22</v>
@@ -2604,7 +2604,7 @@
         <v>65</v>
       </c>
       <c r="C88" s="3" t="n">
-        <v>44324.3985532407</v>
+        <v>44324.5663888889</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>20</v>
@@ -2613,7 +2613,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>22</v>
@@ -2630,7 +2630,7 @@
         <v>65</v>
       </c>
       <c r="C89" s="3" t="n">
-        <v>44324.4017361111</v>
+        <v>44324.5695949074</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>20</v>
@@ -2639,7 +2639,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>22</v>
@@ -2656,7 +2656,7 @@
         <v>65</v>
       </c>
       <c r="C90" s="3" t="n">
-        <v>44324.4025578704</v>
+        <v>44324.5697569444</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>20</v>
@@ -2665,7 +2665,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>22</v>
@@ -2682,7 +2682,7 @@
         <v>65</v>
       </c>
       <c r="C91" s="3" t="n">
-        <v>44324.5663888889</v>
+        <v>44324.5702314815</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>20</v>
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>22</v>
@@ -2708,7 +2708,7 @@
         <v>65</v>
       </c>
       <c r="C92" s="3" t="n">
-        <v>44324.5695949074</v>
+        <v>44324.5710763889</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>20</v>
@@ -2717,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>22</v>
@@ -2734,7 +2734,7 @@
         <v>65</v>
       </c>
       <c r="C93" s="3" t="n">
-        <v>44324.5697569444</v>
+        <v>44324.5753125</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>20</v>
@@ -2743,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>22</v>
@@ -2760,7 +2760,7 @@
         <v>65</v>
       </c>
       <c r="C94" s="3" t="n">
-        <v>44324.5702314815</v>
+        <v>44324.5779861111</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>20</v>
@@ -2769,7 +2769,7 @@
         <v>1</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G94" s="4" t="s">
         <v>22</v>
@@ -2786,7 +2786,7 @@
         <v>65</v>
       </c>
       <c r="C95" s="3" t="n">
-        <v>44324.5710763889</v>
+        <v>44324.5793055556</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>20</v>
@@ -2795,7 +2795,7 @@
         <v>1</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G95" s="4" t="s">
         <v>22</v>
@@ -2812,7 +2812,7 @@
         <v>65</v>
       </c>
       <c r="C96" s="3" t="n">
-        <v>44324.5753125</v>
+        <v>44324.5833101852</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>20</v>
@@ -2821,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>22</v>
@@ -2838,7 +2838,7 @@
         <v>65</v>
       </c>
       <c r="C97" s="3" t="n">
-        <v>44324.5779861111</v>
+        <v>44324.5867824074</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>20</v>
@@ -2847,7 +2847,7 @@
         <v>1</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G97" s="4" t="s">
         <v>22</v>
@@ -2864,7 +2864,7 @@
         <v>65</v>
       </c>
       <c r="C98" s="3" t="n">
-        <v>44324.5793055556</v>
+        <v>44324.5935416667</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>20</v>
@@ -2873,7 +2873,7 @@
         <v>1</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>22</v>
@@ -2890,7 +2890,7 @@
         <v>65</v>
       </c>
       <c r="C99" s="3" t="n">
-        <v>44324.5833101852</v>
+        <v>44324.6890972222</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>20</v>
@@ -2899,7 +2899,7 @@
         <v>1</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="G99" s="4" t="s">
         <v>22</v>
@@ -2916,7 +2916,7 @@
         <v>65</v>
       </c>
       <c r="C100" s="3" t="n">
-        <v>44324.5867824074</v>
+        <v>44324.6902662037</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>20</v>
@@ -2925,7 +2925,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>22</v>
@@ -2942,7 +2942,7 @@
         <v>65</v>
       </c>
       <c r="C101" s="3" t="n">
-        <v>44324.5935416667</v>
+        <v>44324.6906481481</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>20</v>
@@ -2951,7 +2951,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="G101" s="4" t="s">
         <v>22</v>
@@ -2968,7 +2968,7 @@
         <v>65</v>
       </c>
       <c r="C102" s="3" t="n">
-        <v>44324.6890972222</v>
+        <v>44324.6909143519</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>20</v>
@@ -2977,7 +2977,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G102" s="4" t="s">
         <v>22</v>
@@ -2994,7 +2994,7 @@
         <v>65</v>
       </c>
       <c r="C103" s="3" t="n">
-        <v>44324.6902662037</v>
+        <v>44324.6913194444</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>20</v>
@@ -3003,7 +3003,7 @@
         <v>1</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="G103" s="4" t="s">
         <v>22</v>
@@ -3020,7 +3020,7 @@
         <v>65</v>
       </c>
       <c r="C104" s="3" t="n">
-        <v>44324.6906481481</v>
+        <v>44324.6937037037</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>20</v>
@@ -3029,7 +3029,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>22</v>
@@ -3046,7 +3046,7 @@
         <v>65</v>
       </c>
       <c r="C105" s="3" t="n">
-        <v>44324.6909143519</v>
+        <v>44324.6951736111</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>20</v>
@@ -3055,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G105" s="4" t="s">
         <v>22</v>
@@ -3072,7 +3072,7 @@
         <v>65</v>
       </c>
       <c r="C106" s="3" t="n">
-        <v>44324.6913194444</v>
+        <v>44324.6963194444</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>20</v>
@@ -3081,7 +3081,7 @@
         <v>1</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G106" s="4" t="s">
         <v>22</v>
@@ -3098,7 +3098,7 @@
         <v>65</v>
       </c>
       <c r="C107" s="3" t="n">
-        <v>44324.6937037037</v>
+        <v>44324.6994212963</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>20</v>
@@ -3107,7 +3107,7 @@
         <v>1</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>22</v>
@@ -3124,7 +3124,7 @@
         <v>65</v>
       </c>
       <c r="C108" s="3" t="n">
-        <v>44324.6951736111</v>
+        <v>44324.7026851852</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>20</v>
@@ -3133,7 +3133,7 @@
         <v>1</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G108" s="4" t="s">
         <v>22</v>
@@ -3150,7 +3150,7 @@
         <v>65</v>
       </c>
       <c r="C109" s="3" t="n">
-        <v>44324.6963194444</v>
+        <v>44324.7035300926</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>20</v>
@@ -3159,7 +3159,7 @@
         <v>1</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G109" s="4" t="s">
         <v>22</v>
@@ -3176,7 +3176,7 @@
         <v>65</v>
       </c>
       <c r="C110" s="3" t="n">
-        <v>44324.6994212963</v>
+        <v>44324.7393171296</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>20</v>
@@ -3185,7 +3185,7 @@
         <v>1</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G110" s="4" t="s">
         <v>22</v>
@@ -3202,7 +3202,7 @@
         <v>65</v>
       </c>
       <c r="C111" s="3" t="n">
-        <v>44324.7026851852</v>
+        <v>44325.2342361111</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>20</v>
@@ -3211,7 +3211,7 @@
         <v>1</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G111" s="4" t="s">
         <v>22</v>
@@ -3228,7 +3228,7 @@
         <v>65</v>
       </c>
       <c r="C112" s="3" t="n">
-        <v>44324.7035300926</v>
+        <v>44325.2357986111</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>20</v>
@@ -3237,7 +3237,7 @@
         <v>1</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="G112" s="4" t="s">
         <v>22</v>
@@ -3254,7 +3254,7 @@
         <v>65</v>
       </c>
       <c r="C113" s="3" t="n">
-        <v>44324.7393171296</v>
+        <v>44325.236087963</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>20</v>
@@ -3263,7 +3263,7 @@
         <v>1</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G113" s="4" t="s">
         <v>22</v>
@@ -3272,84 +3272,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C114" s="3" t="n">
-        <v>44325.2342361111</v>
-      </c>
-      <c r="D114" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E114" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F114" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G114" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H114" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C115" s="3" t="n">
-        <v>44325.2357986111</v>
-      </c>
-      <c r="D115" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E115" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F115" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G115" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H115" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C116" s="3" t="n">
-        <v>44325.236087963</v>
-      </c>
-      <c r="D116" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E116" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F116" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G116" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H116" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>

</xml_diff>

<commit_message>
changes to test file to test more edge cases
</commit_message>
<xml_diff>
--- a/src/main/resources/testFile.xlsx
+++ b/src/main/resources/testFile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="75">
   <si>
     <t xml:space="preserve">Report Title:</t>
   </si>
@@ -31,19 +31,19 @@
     <t xml:space="preserve">Filter:</t>
   </si>
   <si>
-    <t xml:space="preserve">Vendor/Company Name = 'SECURITAS' AND First Name Is Not Blank AND Last Name Is Not Blank AND Contractor/Vendor Number Begins With 'STUART BRACE' AND Event Date &gt;= '20210508 5:02:46 AM' AND Event Date &lt;= '20210509 6:32:46 AM'</t>
+    <t xml:space="preserve">Vendor/Company Name = 'SECURITAS' AND First Name Is Not Blank AND Last Name Is Not Blank AND Contractor/Vendor Number Begins With 'STUART BRACE' AND Event Date &gt;= '20210524 4:19:34 AM' AND Event Date &lt;= '20210525 12:19:34 PM'</t>
   </si>
   <si>
     <t xml:space="preserve">Report Date:</t>
   </si>
   <si>
-    <t xml:space="preserve">5/9/2021 6:36:54 AM</t>
+    <t xml:space="preserve">5/31/2021 6:23:19 PM</t>
   </si>
   <si>
     <t xml:space="preserve">Record Count:</t>
   </si>
   <si>
-    <t xml:space="preserve">103</t>
+    <t xml:space="preserve">137</t>
   </si>
   <si>
     <t xml:space="preserve">Exported By:</t>
@@ -85,15 +85,18 @@
     <t xml:space="preserve">Contractor </t>
   </si>
   <si>
+    <t xml:space="preserve">PLA0101 - Barrier IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Securitas - S Brace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stuart Brace</t>
+  </si>
+  <si>
     <t xml:space="preserve">PLA0102 - Turnstile West IN</t>
   </si>
   <si>
-    <t xml:space="preserve">Securitas - S Brace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stuart Brace</t>
-  </si>
-  <si>
     <t xml:space="preserve">PLA0112 - B18 Office Main</t>
   </si>
   <si>
@@ -106,18 +109,39 @@
     <t xml:space="preserve">Capes</t>
   </si>
   <si>
-    <t xml:space="preserve">PLA0101 - Barrier IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basharat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iqbal</t>
+    <t xml:space="preserve">Dean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colquhoun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECURITAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0901 - Turnstile South IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STUART BRACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0906 - Sec Office Reception</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI0904 - Turnstile North OUT</t>
   </si>
   <si>
+    <t xml:space="preserve">Derek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devlin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fesal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thames LSI0903 - Turnstile North IN</t>
   </si>
   <si>
@@ -127,103 +151,100 @@
     <t xml:space="preserve">DOGRA</t>
   </si>
   <si>
-    <t xml:space="preserve">SECURITAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STUART BRACE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kayode</t>
   </si>
   <si>
     <t xml:space="preserve">Dairo</t>
   </si>
   <si>
+    <t xml:space="preserve">Thames LSI0604 - 2nd Floor West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0601 - 1st Floor East</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0602 - 1st Floor Central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0303 - Empl East Turnstile IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0306 - Reception Dr In/Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0302 - Empl W Turnstile OUT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thames LSI1202 - TIE Vehicle IN</t>
   </si>
   <si>
-    <t xml:space="preserve">Thames LSI0901 - Turnstile South IN</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thames LSI0501 - HR Office East</t>
   </si>
   <si>
+    <t xml:space="preserve">Thames LSI0305 - Reception Spiral In/Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0401 - Project Area West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0802 - Unit 12A In/Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0801 - Unit 12 In/Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0208 - 1st Floor R&amp;T Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0902 - Turnstile South OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0307 - Empl Car Pk Barrier IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0308 - Empl Cr Pk Barrier OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coulibaly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0702 - Weighbridge OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omoogbolahan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adeola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reehad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI0701 - Weighbridge IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tahiru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haruna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thames LSI1201 - TIE Turnstile IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zubair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thames LSI0502 - HR Office West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0304 - Empl E Turnstile OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0301 - Empl West Turnstile IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0305 - Reception Spiral In/Out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0401 - Project Area West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0604 - 2nd Floor West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0601 - 1st Floor East</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0602 - 1st Floor Central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0802 - Unit 12A In/Out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0801 - Unit 12 In/Out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0208 - 1st Floor R&amp;T Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0902 - Turnstile South OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0307 - Empl Car Pk Barrier IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0308 - Empl Cr Pk Barrier OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0302 - Empl W Turnstile OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0303 - Empl East Turnstile IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coulibaly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0701 - Weighbridge IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0702 - Weighbridge OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omoogbolahan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adeola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tahiru</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haruna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI1201 - TIE Turnstile IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thames LSI0306 - Reception Dr In/Out</t>
   </si>
 </sst>
 </file>
@@ -335,7 +356,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -348,11 +369,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,11 +460,11 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.85"/>
@@ -516,15 +541,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="n">
-        <v>44323.7399884259</v>
+      <c r="C8" s="5" t="n">
+        <v>44340.7379282407</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>20</v>
@@ -542,15 +567,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="n">
-        <v>44324.2536342593</v>
+      <c r="C9" s="5" t="n">
+        <v>44340.7391203704</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
@@ -559,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>22</v>
@@ -575,8 +600,8 @@
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="n">
-        <v>44324.6619560185</v>
+      <c r="C10" s="5" t="n">
+        <v>44340.8389699074</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>20</v>
@@ -601,8 +626,8 @@
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="n">
-        <v>44324.7394560185</v>
+      <c r="C11" s="5" t="n">
+        <v>44340.8458680556</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>20</v>
@@ -620,15 +645,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="n">
-        <v>44324.7423726852</v>
+      <c r="C12" s="5" t="n">
+        <v>44340.8514583333</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>20</v>
@@ -637,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>22</v>
@@ -646,15 +671,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="3" t="n">
-        <v>44325.2423611111</v>
+      <c r="C13" s="5" t="n">
+        <v>44341.0562615741</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>20</v>
@@ -663,7 +688,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>22</v>
@@ -674,13 +699,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>44324.2404861111</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>44341.063125</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>20</v>
@@ -698,76 +723,76 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>44341.0685300926</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="G15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>44341.2429166667</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="3" t="n">
-        <v>44324.75</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="C17" s="5" t="n">
+        <v>44340.2440856481</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="3" t="n">
-        <v>44324.7359837963</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>44324.8191550926</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>22</v>
@@ -778,117 +803,117 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="3" t="n">
-        <v>44324.8323263889</v>
+        <v>30</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>44340.2499768519</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="n">
-        <v>44325.0769791667</v>
+        <v>30</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>44340.7377083333</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="3" t="n">
-        <v>44325.09125</v>
+        <v>30</v>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>44340.7465393519</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="3" t="n">
-        <v>44325.2371180556</v>
+        <v>30</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>44340.7609490741</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="3" t="n">
-        <v>44324.2481365741</v>
+        <v>37</v>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>44340.3540740741</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>20</v>
@@ -897,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>22</v>
@@ -906,15 +931,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="3" t="n">
-        <v>44324.2919328704</v>
+        <v>37</v>
+      </c>
+      <c r="C23" s="5" t="n">
+        <v>44340.7474884259</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>20</v>
@@ -923,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>22</v>
@@ -934,13 +959,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="3" t="n">
-        <v>44324.7502662037</v>
+        <v>37</v>
+      </c>
+      <c r="C24" s="5" t="n">
+        <v>44341.2378356481</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>20</v>
@@ -949,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>22</v>
@@ -960,13 +985,13 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="3" t="n">
-        <v>44325.2498611111</v>
+        <v>39</v>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>44341.2488078704</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>20</v>
@@ -975,154 +1000,154 @@
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="5" t="n">
+        <v>44340.2513888889</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="3" t="n">
-        <v>44325.7498611111</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>44340.7410532407</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="3" t="n">
-        <v>44324.246412037</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="5" t="n">
+        <v>44341.2530208333</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="3" t="n">
-        <v>44324.7481134259</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="3" t="n">
-        <v>44324.7514467593</v>
+        <v>44</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <v>44340.1806018519</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="3" t="n">
-        <v>44325.2491550926</v>
+        <v>44</v>
+      </c>
+      <c r="C30" s="5" t="n">
+        <v>44340.1825462963</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="3" t="n">
-        <v>44324.2345601852</v>
+        <v>44</v>
+      </c>
+      <c r="C31" s="5" t="n">
+        <v>44340.1841782407</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>20</v>
@@ -1131,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>22</v>
@@ -1142,13 +1167,13 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="3" t="n">
-        <v>44324.7356944444</v>
+        <v>44</v>
+      </c>
+      <c r="C32" s="5" t="n">
+        <v>44340.2278935185</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>20</v>
@@ -1157,7 +1182,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>22</v>
@@ -1168,13 +1193,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="3" t="n">
-        <v>44324.739375</v>
+        <v>44</v>
+      </c>
+      <c r="C33" s="5" t="n">
+        <v>44340.2284606481</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>20</v>
@@ -1183,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>22</v>
@@ -1194,13 +1219,13 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="3" t="n">
-        <v>44324.8677314815</v>
+        <v>44</v>
+      </c>
+      <c r="C34" s="5" t="n">
+        <v>44340.228900463</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>20</v>
@@ -1209,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>22</v>
@@ -1220,13 +1245,13 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="3" t="n">
-        <v>44324.8735416667</v>
+        <v>44</v>
+      </c>
+      <c r="C35" s="5" t="n">
+        <v>44340.2355324074</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>20</v>
@@ -1235,7 +1260,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>22</v>
@@ -1246,13 +1271,13 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="3" t="n">
-        <v>44324.8756018519</v>
+        <v>44</v>
+      </c>
+      <c r="C36" s="5" t="n">
+        <v>44340.742974537</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>20</v>
@@ -1261,7 +1286,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>22</v>
@@ -1272,13 +1297,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="3" t="n">
-        <v>44324.8761805556</v>
+        <v>44</v>
+      </c>
+      <c r="C37" s="5" t="n">
+        <v>44340.7448726852</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>20</v>
@@ -1287,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>22</v>
@@ -1298,13 +1323,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="3" t="n">
-        <v>44324.8838773148</v>
+        <v>44</v>
+      </c>
+      <c r="C38" s="5" t="n">
+        <v>44340.8461805556</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>20</v>
@@ -1313,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>22</v>
@@ -1324,13 +1349,13 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="3" t="n">
-        <v>44324.8871643519</v>
+        <v>44</v>
+      </c>
+      <c r="C39" s="5" t="n">
+        <v>44340.8562615741</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>20</v>
@@ -1339,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>22</v>
@@ -1350,13 +1375,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="3" t="n">
-        <v>44324.891087963</v>
+        <v>44</v>
+      </c>
+      <c r="C40" s="5" t="n">
+        <v>44340.8576967593</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>20</v>
@@ -1365,7 +1390,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>22</v>
@@ -1376,13 +1401,13 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="3" t="n">
-        <v>44324.8930671296</v>
+        <v>44</v>
+      </c>
+      <c r="C41" s="5" t="n">
+        <v>44340.8581944444</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>20</v>
@@ -1391,7 +1416,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>22</v>
@@ -1402,13 +1427,13 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="3" t="n">
-        <v>44324.8947337963</v>
+        <v>44</v>
+      </c>
+      <c r="C42" s="5" t="n">
+        <v>44340.8593634259</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>20</v>
@@ -1417,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>22</v>
@@ -1428,13 +1453,13 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="3" t="n">
-        <v>44324.9606481481</v>
+        <v>44</v>
+      </c>
+      <c r="C43" s="5" t="n">
+        <v>44340.8599652778</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>20</v>
@@ -1443,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>22</v>
@@ -1454,13 +1479,13 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="3" t="n">
-        <v>44324.9623611111</v>
+        <v>44</v>
+      </c>
+      <c r="C44" s="5" t="n">
+        <v>44340.8649884259</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>20</v>
@@ -1469,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>22</v>
@@ -1480,13 +1505,13 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="3" t="n">
-        <v>44324.9653703704</v>
+        <v>44</v>
+      </c>
+      <c r="C45" s="5" t="n">
+        <v>44340.8669212963</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>20</v>
@@ -1495,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>22</v>
@@ -1506,13 +1531,13 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="3" t="n">
-        <v>44324.9690509259</v>
+        <v>44</v>
+      </c>
+      <c r="C46" s="5" t="n">
+        <v>44340.8697106481</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>20</v>
@@ -1521,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>22</v>
@@ -1532,13 +1557,13 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="3" t="n">
-        <v>44324.974375</v>
+        <v>44</v>
+      </c>
+      <c r="C47" s="5" t="n">
+        <v>44340.9333217593</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>20</v>
@@ -1547,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>22</v>
@@ -1558,13 +1583,13 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C48" s="3" t="n">
-        <v>44325.0288425926</v>
+        <v>44</v>
+      </c>
+      <c r="C48" s="5" t="n">
+        <v>44340.9350578704</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>20</v>
@@ -1573,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>22</v>
@@ -1584,13 +1609,13 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="3" t="n">
-        <v>44325.1437268518</v>
+        <v>44</v>
+      </c>
+      <c r="C49" s="5" t="n">
+        <v>44340.9377430556</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>20</v>
@@ -1599,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>22</v>
@@ -1610,13 +1635,13 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C50" s="3" t="n">
-        <v>44325.1486458333</v>
+        <v>44</v>
+      </c>
+      <c r="C50" s="5" t="n">
+        <v>44340.9416203704</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>20</v>
@@ -1636,13 +1661,13 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="3" t="n">
-        <v>44325.1714814815</v>
+        <v>44</v>
+      </c>
+      <c r="C51" s="5" t="n">
+        <v>44340.9470486111</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>20</v>
@@ -1651,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>22</v>
@@ -1662,13 +1687,13 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52" s="3" t="n">
-        <v>44325.1767013889</v>
+        <v>44</v>
+      </c>
+      <c r="C52" s="5" t="n">
+        <v>44341.0060300926</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>20</v>
@@ -1677,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>22</v>
@@ -1688,13 +1713,13 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C53" s="3" t="n">
-        <v>44325.177349537</v>
+        <v>44</v>
+      </c>
+      <c r="C53" s="5" t="n">
+        <v>44341.1601736111</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>20</v>
@@ -1703,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>22</v>
@@ -1714,13 +1739,13 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C54" s="3" t="n">
-        <v>44325.1797337963</v>
+        <v>44</v>
+      </c>
+      <c r="C54" s="5" t="n">
+        <v>44341.1646643519</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>20</v>
@@ -1729,7 +1754,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>22</v>
@@ -1740,13 +1765,13 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C55" s="3" t="n">
-        <v>44325.1814236111</v>
+        <v>44</v>
+      </c>
+      <c r="C55" s="5" t="n">
+        <v>44341.1746064815</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>20</v>
@@ -1755,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>22</v>
@@ -1766,13 +1791,13 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C56" s="3" t="n">
-        <v>44325.1848148148</v>
+        <v>44</v>
+      </c>
+      <c r="C56" s="5" t="n">
+        <v>44341.1790393519</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>20</v>
@@ -1781,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>22</v>
@@ -1792,13 +1817,13 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" s="3" t="n">
-        <v>44325.1870138889</v>
+        <v>44</v>
+      </c>
+      <c r="C57" s="5" t="n">
+        <v>44341.1795717593</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>20</v>
@@ -1818,13 +1843,13 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C58" s="3" t="n">
-        <v>44325.1889814815</v>
+        <v>44</v>
+      </c>
+      <c r="C58" s="5" t="n">
+        <v>44341.1800578704</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>20</v>
@@ -1844,13 +1869,13 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C59" s="3" t="n">
-        <v>44325.2369791667</v>
+        <v>44</v>
+      </c>
+      <c r="C59" s="5" t="n">
+        <v>44341.1819097222</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>20</v>
@@ -1859,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>22</v>
@@ -1870,13 +1895,13 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="3" t="n">
-        <v>44324.2438310185</v>
+        <v>44</v>
+      </c>
+      <c r="C60" s="5" t="n">
+        <v>44341.1820949074</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>20</v>
@@ -1885,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>22</v>
@@ -1896,13 +1921,13 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C61" s="3" t="n">
-        <v>44324.7376388889</v>
+        <v>44</v>
+      </c>
+      <c r="C61" s="5" t="n">
+        <v>44341.1841087963</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>20</v>
@@ -1911,7 +1936,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>22</v>
@@ -1922,13 +1947,13 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C62" s="3" t="n">
-        <v>44325.2382986111</v>
+        <v>44</v>
+      </c>
+      <c r="C62" s="5" t="n">
+        <v>44341.1841782407</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>20</v>
@@ -1937,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>22</v>
@@ -1948,169 +1973,169 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="3" t="n">
-        <v>44324.2443171296</v>
+        <v>44</v>
+      </c>
+      <c r="C63" s="5" t="n">
+        <v>44341.1847453704</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="3" t="n">
-        <v>44324.248912037</v>
+        <v>44</v>
+      </c>
+      <c r="C64" s="5" t="n">
+        <v>44341.1876388889</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C65" s="3" t="n">
-        <v>44324.7090856481</v>
+        <v>44</v>
+      </c>
+      <c r="C65" s="5" t="n">
+        <v>44341.1895601852</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" s="3" t="n">
-        <v>44324.7258796296</v>
+        <v>44</v>
+      </c>
+      <c r="C66" s="5" t="n">
+        <v>44341.1910532407</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="3" t="n">
-        <v>44325.2415046296</v>
+        <v>44</v>
+      </c>
+      <c r="C67" s="5" t="n">
+        <v>44341.2286574074</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C68" s="3" t="n">
-        <v>44325.2459837963</v>
+        <v>44</v>
+      </c>
+      <c r="C68" s="5" t="n">
+        <v>44341.2290856481</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C69" s="3" t="n">
-        <v>44324.2283101852</v>
+        <v>44</v>
+      </c>
+      <c r="C69" s="5" t="n">
+        <v>44341.2296527778</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>20</v>
@@ -2119,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>22</v>
@@ -2130,13 +2155,13 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C70" s="3" t="n">
-        <v>44324.2298611111</v>
+        <v>44</v>
+      </c>
+      <c r="C70" s="5" t="n">
+        <v>44341.2411921296</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>20</v>
@@ -2145,7 +2170,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>22</v>
@@ -2156,13 +2181,13 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C71" s="3" t="n">
-        <v>44324.2525</v>
+        <v>62</v>
+      </c>
+      <c r="C71" s="5" t="n">
+        <v>44341.2467013889</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>20</v>
@@ -2171,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>22</v>
@@ -2187,23 +2212,23 @@
       <c r="B72" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="3" t="n">
-        <v>44324.2533564815</v>
+      <c r="C72" s="5" t="n">
+        <v>44340.2538773148</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,34 +2238,34 @@
       <c r="B73" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="3" t="n">
-        <v>44324.2536458333</v>
+      <c r="C73" s="5" t="n">
+        <v>44340.2583333333</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C74" s="3" t="n">
-        <v>44324.2545601852</v>
+        <v>67</v>
+      </c>
+      <c r="C74" s="5" t="n">
+        <v>44340.2469444444</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>20</v>
@@ -2249,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>22</v>
@@ -2260,13 +2285,13 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C75" s="3" t="n">
-        <v>44324.2553472222</v>
+        <v>67</v>
+      </c>
+      <c r="C75" s="5" t="n">
+        <v>44340.2522916667</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>20</v>
@@ -2275,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>22</v>
@@ -2286,13 +2311,13 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C76" s="3" t="n">
-        <v>44324.2562152778</v>
+        <v>67</v>
+      </c>
+      <c r="C76" s="5" t="n">
+        <v>44340.746087963</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>20</v>
@@ -2301,7 +2326,7 @@
         <v>1</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>22</v>
@@ -2312,13 +2337,13 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C77" s="3" t="n">
-        <v>44324.3742013889</v>
+        <v>67</v>
+      </c>
+      <c r="C77" s="5" t="n">
+        <v>44340.7510648148</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>20</v>
@@ -2327,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>22</v>
@@ -2338,13 +2363,13 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C78" s="3" t="n">
-        <v>44324.375625</v>
+        <v>67</v>
+      </c>
+      <c r="C78" s="5" t="n">
+        <v>44341.2448842593</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>20</v>
@@ -2353,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>22</v>
@@ -2364,13 +2389,13 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C79" s="3" t="n">
-        <v>44324.3760416667</v>
+        <v>67</v>
+      </c>
+      <c r="C79" s="5" t="n">
+        <v>44341.2466319444</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>20</v>
@@ -2379,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>22</v>
@@ -2390,13 +2415,13 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C80" s="3" t="n">
-        <v>44324.3765393519</v>
+        <v>70</v>
+      </c>
+      <c r="C80" s="5" t="n">
+        <v>44340.227337963</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>20</v>
@@ -2405,7 +2430,7 @@
         <v>1</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>22</v>
@@ -2416,13 +2441,13 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C81" s="3" t="n">
-        <v>44324.3770138889</v>
+        <v>70</v>
+      </c>
+      <c r="C81" s="5" t="n">
+        <v>44340.2287384259</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>20</v>
@@ -2431,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>22</v>
@@ -2442,13 +2467,13 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C82" s="3" t="n">
-        <v>44324.3917592593</v>
+        <v>70</v>
+      </c>
+      <c r="C82" s="5" t="n">
+        <v>44340.2541782407</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>20</v>
@@ -2457,7 +2482,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>22</v>
@@ -2468,13 +2493,13 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C83" s="3" t="n">
-        <v>44324.3940625</v>
+        <v>70</v>
+      </c>
+      <c r="C83" s="5" t="n">
+        <v>44340.2547222222</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>20</v>
@@ -2483,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>22</v>
@@ -2494,13 +2519,13 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C84" s="3" t="n">
-        <v>44324.3952314815</v>
+        <v>70</v>
+      </c>
+      <c r="C84" s="5" t="n">
+        <v>44340.2559027778</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>20</v>
@@ -2520,13 +2545,13 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C85" s="3" t="n">
-        <v>44324.3985532407</v>
+        <v>70</v>
+      </c>
+      <c r="C85" s="5" t="n">
+        <v>44340.2564236111</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>20</v>
@@ -2535,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>22</v>
@@ -2546,13 +2571,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C86" s="3" t="n">
-        <v>44324.4017361111</v>
+        <v>70</v>
+      </c>
+      <c r="C86" s="5" t="n">
+        <v>44340.2848726852</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>20</v>
@@ -2561,7 +2586,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>22</v>
@@ -2572,13 +2597,13 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C87" s="3" t="n">
-        <v>44324.4025578704</v>
+        <v>70</v>
+      </c>
+      <c r="C87" s="5" t="n">
+        <v>44340.5283101852</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>20</v>
@@ -2587,7 +2612,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>22</v>
@@ -2598,13 +2623,13 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C88" s="3" t="n">
-        <v>44324.5663888889</v>
+        <v>70</v>
+      </c>
+      <c r="C88" s="5" t="n">
+        <v>44340.5284837963</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>20</v>
@@ -2613,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>22</v>
@@ -2624,13 +2649,13 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C89" s="3" t="n">
-        <v>44324.5695949074</v>
+        <v>70</v>
+      </c>
+      <c r="C89" s="5" t="n">
+        <v>44340.5821643519</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>20</v>
@@ -2639,7 +2664,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>22</v>
@@ -2650,13 +2675,13 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C90" s="3" t="n">
-        <v>44324.5697569444</v>
+        <v>70</v>
+      </c>
+      <c r="C90" s="5" t="n">
+        <v>44340.5855439815</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>20</v>
@@ -2665,7 +2690,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>22</v>
@@ -2676,13 +2701,13 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C91" s="3" t="n">
-        <v>44324.5702314815</v>
+        <v>70</v>
+      </c>
+      <c r="C91" s="5" t="n">
+        <v>44340.7448958333</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>20</v>
@@ -2691,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>22</v>
@@ -2702,13 +2727,13 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C92" s="3" t="n">
-        <v>44324.5710763889</v>
+        <v>70</v>
+      </c>
+      <c r="C92" s="5" t="n">
+        <v>44341.2390393519</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>20</v>
@@ -2717,7 +2742,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>22</v>
@@ -2728,13 +2753,13 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C93" s="3" t="n">
-        <v>44324.5753125</v>
+        <v>70</v>
+      </c>
+      <c r="C93" s="5" t="n">
+        <v>44341.2404166667</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>20</v>
@@ -2743,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>22</v>
@@ -2754,13 +2779,13 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C94" s="3" t="n">
-        <v>44324.5779861111</v>
+        <v>70</v>
+      </c>
+      <c r="C94" s="5" t="n">
+        <v>44341.2518981481</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>20</v>
@@ -2780,13 +2805,13 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C95" s="3" t="n">
-        <v>44324.5793055556</v>
+        <v>70</v>
+      </c>
+      <c r="C95" s="5" t="n">
+        <v>44341.2525694444</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>20</v>
@@ -2806,13 +2831,13 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C96" s="3" t="n">
-        <v>44324.5833101852</v>
+        <v>70</v>
+      </c>
+      <c r="C96" s="5" t="n">
+        <v>44341.2537615741</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>20</v>
@@ -2821,7 +2846,7 @@
         <v>1</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>22</v>
@@ -2832,13 +2857,13 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C97" s="3" t="n">
-        <v>44324.5867824074</v>
+        <v>70</v>
+      </c>
+      <c r="C97" s="5" t="n">
+        <v>44341.2543981482</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>20</v>
@@ -2847,7 +2872,7 @@
         <v>1</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G97" s="4" t="s">
         <v>22</v>
@@ -2858,13 +2883,13 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C98" s="3" t="n">
-        <v>44324.5935416667</v>
+        <v>70</v>
+      </c>
+      <c r="C98" s="5" t="n">
+        <v>44341.2544560185</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>20</v>
@@ -2873,7 +2898,7 @@
         <v>1</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>22</v>
@@ -2884,13 +2909,13 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C99" s="3" t="n">
-        <v>44324.6890972222</v>
+        <v>73</v>
+      </c>
+      <c r="C99" s="5" t="n">
+        <v>44340.2827662037</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>20</v>
@@ -2899,7 +2924,7 @@
         <v>1</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G99" s="4" t="s">
         <v>22</v>
@@ -2910,13 +2935,13 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C100" s="3" t="n">
-        <v>44324.6902662037</v>
+        <v>73</v>
+      </c>
+      <c r="C100" s="5" t="n">
+        <v>44340.2830324074</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>20</v>
@@ -2925,7 +2950,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>22</v>
@@ -2936,13 +2961,13 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C101" s="3" t="n">
-        <v>44324.6906481481</v>
+        <v>73</v>
+      </c>
+      <c r="C101" s="5" t="n">
+        <v>44340.2855555556</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>20</v>
@@ -2951,7 +2976,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="G101" s="4" t="s">
         <v>22</v>
@@ -2962,13 +2987,13 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C102" s="3" t="n">
-        <v>44324.6909143519</v>
+        <v>73</v>
+      </c>
+      <c r="C102" s="5" t="n">
+        <v>44340.2877430556</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>20</v>
@@ -2977,7 +3002,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="G102" s="4" t="s">
         <v>22</v>
@@ -2988,13 +3013,13 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C103" s="3" t="n">
-        <v>44324.6913194444</v>
+        <v>73</v>
+      </c>
+      <c r="C103" s="5" t="n">
+        <v>44340.2890856481</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>20</v>
@@ -3014,13 +3039,13 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C104" s="3" t="n">
-        <v>44324.6937037037</v>
+        <v>73</v>
+      </c>
+      <c r="C104" s="5" t="n">
+        <v>44340.2913194444</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>20</v>
@@ -3029,7 +3054,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>22</v>
@@ -3040,13 +3065,13 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C105" s="3" t="n">
-        <v>44324.6951736111</v>
+        <v>73</v>
+      </c>
+      <c r="C105" s="5" t="n">
+        <v>44340.2935069444</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>20</v>
@@ -3055,7 +3080,7 @@
         <v>1</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G105" s="4" t="s">
         <v>22</v>
@@ -3066,13 +3091,13 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C106" s="3" t="n">
-        <v>44324.6963194444</v>
+        <v>73</v>
+      </c>
+      <c r="C106" s="5" t="n">
+        <v>44340.3058217593</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>20</v>
@@ -3092,13 +3117,13 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C107" s="3" t="n">
-        <v>44324.6994212963</v>
+        <v>73</v>
+      </c>
+      <c r="C107" s="5" t="n">
+        <v>44340.3062268519</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>20</v>
@@ -3107,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>22</v>
@@ -3118,13 +3143,13 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C108" s="3" t="n">
-        <v>44324.7026851852</v>
+        <v>73</v>
+      </c>
+      <c r="C108" s="5" t="n">
+        <v>44340.3500578704</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>20</v>
@@ -3133,7 +3158,7 @@
         <v>1</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G108" s="4" t="s">
         <v>22</v>
@@ -3144,13 +3169,13 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C109" s="3" t="n">
-        <v>44324.7035300926</v>
+        <v>73</v>
+      </c>
+      <c r="C109" s="5" t="n">
+        <v>44340.3508333333</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>20</v>
@@ -3159,7 +3184,7 @@
         <v>1</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G109" s="4" t="s">
         <v>22</v>
@@ -3170,13 +3195,13 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C110" s="3" t="n">
-        <v>44324.7393171296</v>
+        <v>73</v>
+      </c>
+      <c r="C110" s="5" t="n">
+        <v>44340.3755671296</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>20</v>
@@ -3185,7 +3210,7 @@
         <v>1</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="G110" s="4" t="s">
         <v>22</v>
@@ -3196,13 +3221,13 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C111" s="3" t="n">
-        <v>44325.2342361111</v>
+        <v>73</v>
+      </c>
+      <c r="C111" s="5" t="n">
+        <v>44340.3757291667</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>20</v>
@@ -3211,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="G111" s="4" t="s">
         <v>22</v>
@@ -3222,13 +3247,13 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C112" s="3" t="n">
-        <v>44325.2357986111</v>
+        <v>73</v>
+      </c>
+      <c r="C112" s="5" t="n">
+        <v>44340.3852662037</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>20</v>
@@ -3237,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G112" s="4" t="s">
         <v>22</v>
@@ -3248,13 +3273,13 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C113" s="3" t="n">
-        <v>44325.236087963</v>
+        <v>73</v>
+      </c>
+      <c r="C113" s="5" t="n">
+        <v>44340.6082175926</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>20</v>
@@ -3263,7 +3288,7 @@
         <v>1</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G113" s="4" t="s">
         <v>22</v>
@@ -3272,8 +3297,786 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C114" s="5" t="n">
+        <v>44340.6083680556</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H114" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C115" s="5" t="n">
+        <v>44340.6464930556</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G115" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H115" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C116" s="5" t="n">
+        <v>44340.6560185185</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G116" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H116" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C117" s="5" t="n">
+        <v>44340.685775463</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G117" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H117" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C118" s="5" t="n">
+        <v>44340.6859490741</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G118" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H118" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C119" s="5" t="n">
+        <v>44340.7027893519</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G119" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H119" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C120" s="5" t="n">
+        <v>44340.702974537</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G120" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H120" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C121" s="5" t="n">
+        <v>44340.7300231481</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G121" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H121" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C122" s="5" t="n">
+        <v>44340.7302430556</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G122" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H122" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C123" s="5" t="n">
+        <v>44341.2839814815</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G123" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H123" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C124" s="5" t="n">
+        <v>44341.2843171296</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F124" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H124" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C125" s="5" t="n">
+        <v>44341.2864930556</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F125" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G125" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H125" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C126" s="5" t="n">
+        <v>44341.2892708333</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F126" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G126" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H126" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C127" s="5" t="n">
+        <v>44341.2907407407</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G127" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H127" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C128" s="5" t="n">
+        <v>44341.2928472222</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F128" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G128" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H128" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C129" s="5" t="n">
+        <v>44341.2950231481</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F129" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G129" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H129" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C130" s="5" t="n">
+        <v>44341.3069675926</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H130" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C131" s="5" t="n">
+        <v>44341.3071412037</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H131" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C132" s="5" t="n">
+        <v>44341.3298842593</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F132" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G132" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H132" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C133" s="5" t="n">
+        <v>44341.3299884259</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F133" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G133" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H133" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C134" s="5" t="n">
+        <v>44341.3597337963</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E134" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F134" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G134" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H134" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C135" s="5" t="n">
+        <v>44341.3829976852</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F135" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H135" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C136" s="5" t="n">
+        <v>44341.3831712963</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G136" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H136" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C137" s="5" t="n">
+        <v>44341.3919560185</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G137" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H137" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C138" s="5" t="n">
+        <v>44341.4045138889</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F138" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G138" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H138" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C139" s="5" t="n">
+        <v>44341.4271180556</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G139" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H139" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C140" s="5" t="n">
+        <v>44341.4272800926</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F140" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G140" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H140" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C141" s="5" t="n">
+        <v>44341.4275462963</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E141" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F141" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G141" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H141" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C142" s="5" t="n">
+        <v>44341.4277546296</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F142" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G142" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H142" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C143" s="5" t="n">
+        <v>44341.4364236111</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F143" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G143" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H143" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>